<commit_message>
Reword feedback to bar chart
</commit_message>
<xml_diff>
--- a/data_raw/ECT_dict.xlsx
+++ b/data_raw/ECT_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\ECT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CD2BE3-6F40-42EB-8AE0-24AD64553559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B989A5-26A2-4B0C-AA63-8286B5269CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCFEBC1B-561E-412E-A77D-B38079EBE1BD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
   <si>
     <t>key</t>
   </si>
@@ -210,9 +210,6 @@
     <t>INCORRECT</t>
   </si>
   <si>
-    <t>That was incorrect</t>
-  </si>
-  <si>
     <t>Das war leider falsch.</t>
   </si>
   <si>
@@ -292,6 +289,36 @@
   </si>
   <si>
     <t>Frage {{num_question}} out of {{test_length}}.</t>
+  </si>
+  <si>
+    <t>FEEDBACK_SHORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You rated {{num_correct}} out of {{num_questions}} ({{perc_correct}}%) items correctly. </t>
+  </si>
+  <si>
+    <t>Sie haben {{num_correct}} von {{num_questions}} ({{perc_correct}}%) Fragen richtig beantworted.</t>
+  </si>
+  <si>
+    <t>That was incorrect.</t>
+  </si>
+  <si>
+    <t>INCORRECT_RAW</t>
+  </si>
+  <si>
+    <t>Incorrect</t>
+  </si>
+  <si>
+    <t>Richtig</t>
+  </si>
+  <si>
+    <t>CORRECT_RAW</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Falsch</t>
   </si>
 </sst>
 </file>
@@ -340,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -350,6 +377,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -666,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A736F0E7-DA9E-4210-9CD5-212BBAD85A50}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +725,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>31</v>
@@ -709,7 +739,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -780,35 +810,35 @@
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -816,10 +846,10 @@
         <v>60</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -827,7 +857,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>16</v>
@@ -838,10 +868,10 @@
         <v>56</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -849,165 +879,198 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>19</v>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>88</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="3" t="s">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>76</v>
+        <v>53</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>85</v>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed feedback pie chart.
</commit_message>
<xml_diff>
--- a/data_raw/ECT_dict.xlsx
+++ b/data_raw/ECT_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\ECT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B989A5-26A2-4B0C-AA63-8286B5269CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B3547D-189C-4494-B111-A70B99AE56B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCFEBC1B-561E-412E-A77D-B38079EBE1BD}"/>
   </bookViews>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A736F0E7-DA9E-4210-9CD5-212BBAD85A50}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Feedback details. Remove stimulus name from item page.
</commit_message>
<xml_diff>
--- a/data_raw/ECT_dict.xlsx
+++ b/data_raw/ECT_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\ECT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B3547D-189C-4494-B111-A70B99AE56B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A6924D-397D-4B82-902C-7AB48631355F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCFEBC1B-561E-412E-A77D-B38079EBE1BD}"/>
   </bookViews>
@@ -294,12 +294,6 @@
     <t>FEEDBACK_SHORT</t>
   </si>
   <si>
-    <t xml:space="preserve">You rated {{num_correct}} out of {{num_questions}} ({{perc_correct}}%) items correctly. </t>
-  </si>
-  <si>
-    <t>Sie haben {{num_correct}} von {{num_questions}} ({{perc_correct}}%) Fragen richtig beantworted.</t>
-  </si>
-  <si>
     <t>That was incorrect.</t>
   </si>
   <si>
@@ -319,6 +313,12 @@
   </si>
   <si>
     <t>Falsch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You finished the Expressivity Comparison Test with {{num_correct}} out of {{num_questions}} ({{perc_correct}}%) correct answers. </t>
+  </si>
+  <si>
+    <t>Sie haben den Test zum Ausdruck in der Musik mit {{num_correct}} von {{num_questions}} ({{perc_correct}}%) richtigen Antworten beendet.</t>
   </si>
 </sst>
 </file>
@@ -699,7 +699,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD37"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,7 +846,7 @@
         <v>60</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>61</v>
@@ -885,15 +885,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>88</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1053,24 +1053,24 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>